<commit_message>
updating export function and domain table
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="408" windowWidth="22692" windowHeight="8220"/>
+    <workbookView xWindow="290" yWindow="410" windowWidth="22690" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="139">
   <si>
     <t>DWQ WMU</t>
   </si>
@@ -421,6 +421,18 @@
   </si>
   <si>
     <t>SSC_EndMon</t>
+  </si>
+  <si>
+    <t>CriterionType</t>
+  </si>
+  <si>
+    <t>CriterionLabel</t>
+  </si>
+  <si>
+    <t>AsmntAggFun</t>
+  </si>
+  <si>
+    <t>SSC_MLID</t>
   </si>
 </sst>
 </file>
@@ -759,18 +771,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -778,7 +790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -786,7 +798,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -794,7 +806,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -802,7 +814,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -810,7 +822,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -818,7 +830,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -826,7 +838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -834,7 +846,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -842,7 +854,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -850,7 +862,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -858,7 +870,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -866,7 +878,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -874,7 +886,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -882,7 +894,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -890,7 +902,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -898,7 +910,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -906,7 +918,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -914,7 +926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -922,7 +934,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -930,7 +942,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -938,7 +950,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -946,7 +958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -954,7 +966,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -962,7 +974,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -970,7 +982,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -978,7 +990,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -986,7 +998,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>132</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -1058,7 +1070,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1066,7 +1078,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1106,7 +1118,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1122,7 +1134,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -1130,7 +1142,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>121</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -1178,7 +1190,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>124</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +1262,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1294,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -1306,587 +1318,627 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>133</v>
       </c>
-      <c r="B68" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>134</v>
       </c>
-      <c r="B69" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="B73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>43</v>
       </c>
-      <c r="B70" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="B75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>44</v>
       </c>
-      <c r="B71" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="B76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>45</v>
       </c>
-      <c r="B72" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="B77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>46</v>
       </c>
-      <c r="B73" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="B78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>47</v>
       </c>
-      <c r="B74" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="B79" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>48</v>
       </c>
-      <c r="B75" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="B80" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>49</v>
       </c>
-      <c r="B76" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>50</v>
       </c>
-      <c r="B77" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>51</v>
       </c>
-      <c r="B78" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>52</v>
       </c>
-      <c r="B79" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="B84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>53</v>
       </c>
-      <c r="B80" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="B85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>54</v>
       </c>
-      <c r="B81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="B86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>55</v>
       </c>
-      <c r="B82" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>56</v>
       </c>
-      <c r="B83" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B88" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>57</v>
       </c>
-      <c r="B84" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>58</v>
       </c>
-      <c r="B85" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>59</v>
       </c>
-      <c r="B86" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>60</v>
       </c>
-      <c r="B87" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>61</v>
       </c>
-      <c r="B88" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>62</v>
       </c>
-      <c r="B89" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B94" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>126</v>
       </c>
-      <c r="B90" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>127</v>
       </c>
-      <c r="B91" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="B96" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>128</v>
       </c>
-      <c r="B92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="B97" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>129</v>
       </c>
-      <c r="B93" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="B98" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>130</v>
       </c>
-      <c r="B94" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>131</v>
       </c>
-      <c r="B95" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>63</v>
       </c>
-      <c r="B96" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>64</v>
       </c>
-      <c r="B97" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="B102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>65</v>
       </c>
-      <c r="B98" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>66</v>
       </c>
-      <c r="B99" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="B104" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>67</v>
       </c>
-      <c r="B100" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>68</v>
       </c>
-      <c r="B101" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="B106" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>69</v>
       </c>
-      <c r="B102" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="B107" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>70</v>
       </c>
-      <c r="B103" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B108" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>74</v>
       </c>
-      <c r="B104" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="B109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>75</v>
       </c>
-      <c r="B105" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="B110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>76</v>
       </c>
-      <c r="B106" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="B111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>77</v>
       </c>
-      <c r="B107" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="B112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>0</v>
       </c>
-      <c r="B108" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="B113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>78</v>
       </c>
-      <c r="B109" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="B114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>1</v>
       </c>
-      <c r="B110" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="B115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>2</v>
       </c>
-      <c r="B111" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="B116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>79</v>
       </c>
-      <c r="B112" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="B117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>105</v>
       </c>
-      <c r="B113" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="B118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>81</v>
       </c>
-      <c r="B114" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="B119" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>82</v>
       </c>
-      <c r="B115" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="B120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>83</v>
       </c>
-      <c r="B116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="B121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>9</v>
       </c>
-      <c r="B117" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="B122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>10</v>
       </c>
-      <c r="B118" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="B123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>11</v>
       </c>
-      <c r="B119" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="B124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>84</v>
       </c>
-      <c r="B120" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+      <c r="B125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>85</v>
       </c>
-      <c r="B121" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="B126" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>86</v>
       </c>
-      <c r="B122" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="B127" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>23</v>
       </c>
-      <c r="B123" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="B128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>24</v>
       </c>
-      <c r="B124" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+      <c r="B129" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>87</v>
       </c>
-      <c r="B125" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="B130" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>88</v>
       </c>
-      <c r="B126" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="B131" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>89</v>
       </c>
-      <c r="B127" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+      <c r="B132" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>90</v>
       </c>
-      <c r="B128" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>14</v>
       </c>
-      <c r="B129" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="B134" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>91</v>
       </c>
-      <c r="B130" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="B135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>92</v>
       </c>
-      <c r="B131" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+      <c r="B136" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>93</v>
       </c>
-      <c r="B132" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+      <c r="B137" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>94</v>
       </c>
-      <c r="B133" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+      <c r="B138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>95</v>
       </c>
-      <c r="B134" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+      <c r="B139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>96</v>
       </c>
-      <c r="B135" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="B140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>97</v>
       </c>
-      <c r="B136" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+      <c r="B141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>98</v>
       </c>
-      <c r="B137" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+      <c r="B142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>99</v>
       </c>
-      <c r="B138" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+      <c r="B143" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>100</v>
       </c>
-      <c r="B139" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="B144" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>101</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B145" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1903,7 +1955,7 @@
       <selection activeCell="AK2" sqref="A2:AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2029,7 +2081,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all sorts of things
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="290" yWindow="410" windowWidth="22690" windowHeight="8220"/>
+    <workbookView xWindow="288" yWindow="408" windowWidth="22692" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="141">
   <si>
     <t>DWQ WMU</t>
   </si>
@@ -433,6 +433,12 @@
   </si>
   <si>
     <t>SSC_MLID</t>
+  </si>
+  <si>
+    <t>CriterionFormula</t>
+  </si>
+  <si>
+    <t>CalculatedCrit</t>
   </si>
 </sst>
 </file>
@@ -771,18 +777,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B145"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -790,7 +796,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -798,7 +804,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -806,7 +812,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -814,7 +820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -822,7 +828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -830,7 +836,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -838,7 +844,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -846,7 +852,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -854,7 +860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -862,7 +868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -870,7 +876,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -878,7 +884,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -886,7 +892,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -894,7 +900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -902,7 +908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
@@ -910,7 +916,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -918,7 +924,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -926,7 +932,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -934,7 +940,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -942,7 +948,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -950,7 +956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -958,7 +964,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -966,7 +972,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -974,7 +980,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -982,7 +988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -990,7 +996,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1022,7 +1028,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>132</v>
       </c>
@@ -1030,7 +1036,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -1038,7 +1044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -1046,7 +1052,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>121</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>123</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -1190,7 +1196,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -1206,7 +1212,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -1214,7 +1220,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>112</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>124</v>
       </c>
@@ -1246,7 +1252,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>125</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>40</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>41</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>42</v>
       </c>
@@ -1294,7 +1300,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -1302,7 +1308,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>106</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -1326,7 +1332,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -1342,7 +1348,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>133</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -1382,7 +1388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>45</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>46</v>
       </c>
@@ -1406,7 +1412,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>47</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -1422,523 +1428,539 @@
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>49</v>
       </c>
-      <c r="B81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>50</v>
       </c>
-      <c r="B82" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="B84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>51</v>
       </c>
-      <c r="B83" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="B85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>52</v>
       </c>
-      <c r="B84" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="B86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>53</v>
       </c>
-      <c r="B85" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+      <c r="B87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>54</v>
       </c>
-      <c r="B86" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="B88" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>55</v>
       </c>
-      <c r="B87" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="B89" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>56</v>
       </c>
-      <c r="B88" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="B90" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>57</v>
       </c>
-      <c r="B89" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>58</v>
       </c>
-      <c r="B90" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>59</v>
       </c>
-      <c r="B91" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="B93" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>60</v>
       </c>
-      <c r="B92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="B94" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>61</v>
       </c>
-      <c r="B93" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="B95" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>62</v>
       </c>
-      <c r="B94" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="B96" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>126</v>
       </c>
-      <c r="B95" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+      <c r="B97" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>127</v>
       </c>
-      <c r="B96" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="B98" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>128</v>
       </c>
-      <c r="B97" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>129</v>
       </c>
-      <c r="B98" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>130</v>
       </c>
-      <c r="B99" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>131</v>
       </c>
-      <c r="B100" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+      <c r="B102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>63</v>
       </c>
-      <c r="B101" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>64</v>
       </c>
-      <c r="B102" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+      <c r="B104" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>65</v>
       </c>
-      <c r="B103" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>66</v>
       </c>
-      <c r="B104" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+      <c r="B106" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>67</v>
       </c>
-      <c r="B105" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+      <c r="B107" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>68</v>
       </c>
-      <c r="B106" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+      <c r="B108" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>69</v>
       </c>
-      <c r="B107" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+      <c r="B109" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>70</v>
       </c>
-      <c r="B108" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+      <c r="B110" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>74</v>
       </c>
-      <c r="B109" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+      <c r="B111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>75</v>
       </c>
-      <c r="B110" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+      <c r="B112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>76</v>
       </c>
-      <c r="B111" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+      <c r="B113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>77</v>
       </c>
-      <c r="B112" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+      <c r="B114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>0</v>
       </c>
-      <c r="B113" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+      <c r="B115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>78</v>
       </c>
-      <c r="B114" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+      <c r="B116" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>1</v>
       </c>
-      <c r="B115" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+      <c r="B117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>2</v>
       </c>
-      <c r="B116" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+      <c r="B118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>79</v>
       </c>
-      <c r="B117" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+      <c r="B119" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>105</v>
       </c>
-      <c r="B118" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+      <c r="B120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>81</v>
       </c>
-      <c r="B119" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+      <c r="B121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>82</v>
       </c>
-      <c r="B120" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+      <c r="B122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>83</v>
       </c>
-      <c r="B121" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+      <c r="B123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>9</v>
       </c>
-      <c r="B122" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+      <c r="B124" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>10</v>
       </c>
-      <c r="B123" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+      <c r="B125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B124" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+      <c r="B126" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>84</v>
       </c>
-      <c r="B125" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+      <c r="B127" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>85</v>
       </c>
-      <c r="B126" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+      <c r="B128" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>86</v>
       </c>
-      <c r="B127" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+      <c r="B129" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>23</v>
       </c>
-      <c r="B128" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="B130" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>24</v>
       </c>
-      <c r="B129" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="B131" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>87</v>
       </c>
-      <c r="B130" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+      <c r="B132" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>88</v>
       </c>
-      <c r="B131" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>89</v>
       </c>
-      <c r="B132" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="B134" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>90</v>
       </c>
-      <c r="B133" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="B135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>14</v>
       </c>
-      <c r="B134" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+      <c r="B136" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>91</v>
       </c>
-      <c r="B135" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="B137" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>92</v>
       </c>
-      <c r="B136" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+      <c r="B138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>93</v>
       </c>
-      <c r="B137" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+      <c r="B139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>94</v>
       </c>
-      <c r="B138" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+      <c r="B140" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>95</v>
       </c>
-      <c r="B139" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+      <c r="B141" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>96</v>
       </c>
-      <c r="B140" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+      <c r="B142" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>97</v>
       </c>
-      <c r="B141" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+      <c r="B143" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>98</v>
       </c>
-      <c r="B142" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+      <c r="B144" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>99</v>
       </c>
-      <c r="B143" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+      <c r="B145" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>100</v>
       </c>
-      <c r="B144" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+      <c r="B146" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>101</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B147" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1955,7 +1977,7 @@
       <selection activeCell="AK2" sqref="A2:AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -2081,7 +2103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to file formatting, changes to export translation table
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="150">
   <si>
     <t>DWQ WMU</t>
   </si>
@@ -804,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:B146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
         <v>71</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
         <v>71</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
         <v>71</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>71</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
         <v>71</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>71</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>71</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
         <v>71</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
         <v>71</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
         <v>71</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
         <v>71</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>71</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
         <v>71</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
         <v>71</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
         <v>71</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
         <v>71</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B49" t="s">
         <v>71</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
         <v>71</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>22</v>
       </c>
       <c r="B51" t="s">
         <v>71</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
         <v>71</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
         <v>71</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
         <v>71</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
         <v>71</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B56" t="s">
         <v>71</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="B57" t="s">
         <v>71</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
         <v>71</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
         <v>71</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
         <v>71</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
         <v>71</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="B62" t="s">
         <v>71</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
         <v>71</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
         <v>71</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
         <v>71</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B66" t="s">
         <v>71</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B67" t="s">
         <v>71</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
         <v>71</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B69" t="s">
         <v>71</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="B70" t="s">
         <v>71</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="B71" t="s">
         <v>71</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
         <v>71</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
         <v>71</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
         <v>71</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="B76" t="s">
         <v>71</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B77" t="s">
         <v>71</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="B78" t="s">
         <v>71</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
         <v>71</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B80" t="s">
         <v>71</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="B81" t="s">
         <v>71</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B82" t="s">
         <v>71</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B83" t="s">
         <v>71</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B84" t="s">
         <v>71</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B85" t="s">
         <v>71</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
         <v>71</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
         <v>71</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B88" t="s">
         <v>71</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B89" t="s">
         <v>71</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B90" t="s">
         <v>71</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B91" t="s">
         <v>71</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B92" t="s">
         <v>71</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B93" t="s">
         <v>71</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B94" t="s">
         <v>71</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="B95" t="s">
         <v>71</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="B96" t="s">
         <v>71</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B97" t="s">
         <v>71</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B98" t="s">
         <v>71</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B99" t="s">
         <v>71</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B100" t="s">
         <v>71</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="B101" t="s">
         <v>71</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="B102" t="s">
         <v>71</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
         <v>71</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B104" t="s">
         <v>71</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B105" t="s">
         <v>71</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B106" t="s">
         <v>71</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B107" t="s">
         <v>71</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
         <v>71</v>
@@ -1681,23 +1681,23 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B109" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B110" t="s">
-        <v>100</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B111" t="s">
         <v>100</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B112" t="s">
         <v>100</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
       <c r="B113" t="s">
         <v>100</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="B114" t="s">
         <v>100</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>2</v>
+        <v>139</v>
       </c>
       <c r="B115" t="s">
         <v>100</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="B116" t="s">
         <v>100</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="B117" t="s">
         <v>100</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="B118" t="s">
         <v>100</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="B119" t="s">
         <v>100</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="B120" t="s">
         <v>100</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="B121" t="s">
         <v>100</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B122" t="s">
         <v>100</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
         <v>100</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B124" t="s">
         <v>100</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B125" t="s">
         <v>100</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="B126" t="s">
         <v>100</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>142</v>
+        <v>84</v>
       </c>
       <c r="B127" t="s">
         <v>100</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="B128" t="s">
         <v>100</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
         <v>100</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B130" t="s">
         <v>100</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B131" t="s">
         <v>100</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B132" t="s">
         <v>100</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="B133" t="s">
         <v>100</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B134" t="s">
         <v>100</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="B135" t="s">
         <v>100</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B136" t="s">
         <v>100</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B137" t="s">
         <v>100</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B138" t="s">
         <v>100</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="B139" t="s">
         <v>100</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="B140" t="s">
         <v>100</v>
@@ -1937,7 +1937,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B141" t="s">
         <v>100</v>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="B142" t="s">
         <v>100</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B143" t="s">
         <v>100</v>
@@ -1961,9 +1961,25 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>149</v>
+      </c>
+      <c r="B144" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>98</v>
+      </c>
+      <c r="B145" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>99</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to export function
- adding columns and code to accommodate rejected data.
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="168">
   <si>
     <t>DWQ WMU</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>IR_Unit_Comment</t>
+  </si>
+  <si>
+    <t>MonitoringLocationIdentifier</t>
   </si>
 </sst>
 </file>
@@ -855,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1967,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="B138" t="s">
         <v>94</v>
@@ -1972,7 +1975,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B139" t="s">
         <v>94</v>
@@ -1980,7 +1983,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="B140" t="s">
         <v>94</v>
@@ -1988,7 +1991,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B141" t="s">
         <v>94</v>
@@ -1996,7 +1999,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B142" t="s">
         <v>94</v>
@@ -2004,7 +2007,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B143" t="s">
         <v>94</v>
@@ -2012,7 +2015,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B144" t="s">
         <v>94</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B145" t="s">
         <v>94</v>
@@ -2028,7 +2031,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="B146" t="s">
         <v>94</v>
@@ -2036,7 +2039,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="B147" t="s">
         <v>94</v>
@@ -2044,7 +2047,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B148" t="s">
         <v>94</v>
@@ -2052,7 +2055,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B149" t="s">
         <v>94</v>
@@ -2060,7 +2063,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B150" t="s">
         <v>94</v>
@@ -2068,7 +2071,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B151" t="s">
         <v>94</v>
@@ -2076,7 +2079,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B152" t="s">
         <v>94</v>
@@ -2084,7 +2087,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B153" t="s">
         <v>94</v>
@@ -2092,7 +2095,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="B154" t="s">
         <v>94</v>
@@ -2100,7 +2103,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B155" t="s">
         <v>94</v>
@@ -2108,7 +2111,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B156" t="s">
         <v>94</v>
@@ -2116,7 +2119,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B157" t="s">
         <v>94</v>
@@ -2124,7 +2127,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="B158" t="s">
         <v>94</v>
@@ -2132,7 +2135,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="B159" t="s">
         <v>94</v>
@@ -2140,7 +2143,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="B160" t="s">
         <v>94</v>
@@ -2148,7 +2151,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="B161" t="s">
         <v>94</v>
@@ -2156,7 +2159,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="B162" t="s">
         <v>94</v>
@@ -2164,7 +2167,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B163" t="s">
         <v>94</v>
@@ -2172,9 +2175,17 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>92</v>
+      </c>
+      <c r="B164" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>93</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B165" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to export file and columns
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="169">
   <si>
     <t>DWQ WMU</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>MonitoringLocationIdentifier</t>
+  </si>
+  <si>
+    <t>IR_Screen_FLAG</t>
   </si>
 </sst>
 </file>
@@ -858,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B165"/>
+  <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,7 +2106,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="B155" t="s">
         <v>94</v>
@@ -2111,7 +2114,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="B156" t="s">
         <v>94</v>
@@ -2119,7 +2122,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B157" t="s">
         <v>94</v>
@@ -2127,7 +2130,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B158" t="s">
         <v>94</v>
@@ -2135,7 +2138,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B159" t="s">
         <v>94</v>
@@ -2143,7 +2146,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="B160" t="s">
         <v>94</v>
@@ -2151,7 +2154,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="B161" t="s">
         <v>94</v>
@@ -2159,7 +2162,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B162" t="s">
         <v>94</v>
@@ -2167,7 +2170,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="B163" t="s">
         <v>94</v>
@@ -2175,7 +2178,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B164" t="s">
         <v>94</v>
@@ -2183,9 +2186,25 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>142</v>
+      </c>
+      <c r="B165" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>92</v>
+      </c>
+      <c r="B166" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>93</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trying to bar against table join errors between calc rejects and noncalcs
</commit_message>
<xml_diff>
--- a/inst/extdata/IR_export_translations.xlsx
+++ b/inst/extdata/IR_export_translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehinman\Documents\GitHub\irTools\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEA4A6F-5786-4FCA-A0CB-5767526845D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ACFA20-D4B9-4011-9C2E-EC5209588A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="408" windowWidth="19416" windowHeight="8088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="290" yWindow="410" windowWidth="19420" windowHeight="8090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,9 +429,6 @@
     <t>IR_Cat</t>
   </si>
   <si>
-    <t>IRParameterName</t>
-  </si>
-  <si>
     <t>ParameterGroupName</t>
   </si>
   <si>
@@ -538,6 +535,9 @@
   </si>
   <si>
     <t>SS_calc</t>
+  </si>
+  <si>
+    <t>RuleParameterName</t>
   </si>
 </sst>
 </file>
@@ -915,16 +915,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -932,7 +932,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -940,7 +940,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -948,7 +948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -956,23 +956,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>169</v>
       </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>170</v>
-      </c>
       <c r="B6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -980,7 +980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -988,7 +988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -996,7 +996,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1012,15 +1012,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1036,23 +1036,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>163</v>
       </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>164</v>
-      </c>
       <c r="B16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>107</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>106</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1140,23 +1140,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>165</v>
       </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>166</v>
-      </c>
       <c r="B29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>127</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>129</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>124</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -1236,23 +1236,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>128</v>
       </c>
@@ -1260,47 +1260,47 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>139</v>
       </c>
-      <c r="B43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>140</v>
-      </c>
       <c r="B44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>40</v>
       </c>
@@ -1308,31 +1308,31 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>151</v>
       </c>
-      <c r="B49" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>152</v>
       </c>
-      <c r="B50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>153</v>
-      </c>
       <c r="B51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>130</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>131</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -1404,15 +1404,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>21</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -1428,23 +1428,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>156</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>157</v>
       </c>
-      <c r="B64" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>158</v>
-      </c>
       <c r="B65" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>100</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>41</v>
       </c>
@@ -1500,23 +1500,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>143</v>
       </c>
-      <c r="B73" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>144</v>
-      </c>
       <c r="B74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>22</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>109</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>110</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>25</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>111</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -1572,23 +1572,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>145</v>
       </c>
-      <c r="B82" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>146</v>
-      </c>
       <c r="B83" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>27</v>
       </c>
@@ -1596,55 +1596,55 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>147</v>
       </c>
-      <c r="B85" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>148</v>
-      </c>
       <c r="B86" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>159</v>
       </c>
-      <c r="B87" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="B88" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>160</v>
       </c>
-      <c r="B88" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="B89" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>161</v>
       </c>
-      <c r="B89" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>162</v>
-      </c>
       <c r="B90" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>28</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>29</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -1700,15 +1700,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B98" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>32</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>34</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>36</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>116</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>42</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>43</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>44</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>45</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>46</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>47</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>49</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>50</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>51</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>52</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>53</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>54</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>55</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>56</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>58</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>59</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>60</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>61</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>62</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>66</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>67</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>68</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>69</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>132</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>97</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>73</v>
       </c>
@@ -2060,15 +2060,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B143" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>7</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>76</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>77</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>90</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>91</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>95</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>78</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>20</v>
       </c>
@@ -2140,31 +2140,31 @@
         <v>94</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
+        <v>171</v>
+      </c>
+      <c r="B153" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>135</v>
       </c>
-      <c r="B153" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+      <c r="B154" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>136</v>
       </c>
-      <c r="B154" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>137</v>
-      </c>
       <c r="B155" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>127</v>
       </c>
@@ -2172,15 +2172,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B157" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>133</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>79</v>
       </c>
@@ -2196,23 +2196,23 @@
         <v>94</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B160" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B161" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>134</v>
       </c>
@@ -2220,23 +2220,23 @@
         <v>94</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>138</v>
+      </c>
+      <c r="B163" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>139</v>
       </c>
-      <c r="B163" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>140</v>
-      </c>
       <c r="B164" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>128</v>
       </c>
@@ -2244,15 +2244,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B166" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>82</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>12</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>88</v>
       </c>
@@ -2276,15 +2276,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B170" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>92</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>93</v>
       </c>
@@ -2314,9 +2314,9 @@
       <selection activeCell="AK2" sqref="A2:AK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2440,7 +2440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>